<commit_message>
need the Ga part
</commit_message>
<xml_diff>
--- a/Info/Exemplo excel.xlsx
+++ b/Info/Exemplo excel.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\CEAF\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B1B72-BDB7-4786-8F6D-B9BE82482050}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0998B4CD-8E6B-44B8-87D3-732179A282B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{570AC9AF-20DC-488D-8983-B6D091859FF1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{570AC9AF-20DC-488D-8983-B6D091859FF1}"/>
   </bookViews>
   <sheets>
     <sheet name="alunos" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="empresas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -450,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F5DF67-2746-4161-9C91-10A4CD1D25E2}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A8509C-E447-4135-BB59-9CB2AA286235}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>